<commit_message>
Started implementing intermediate representation
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -94,26 +94,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,32 +170,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -220,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -506,79 +488,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="11:13" x14ac:dyDescent="0.3">
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="26" spans="11:13" x14ac:dyDescent="0.3">
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>